<commit_message>
Uppdaterad verision av excel -> matlab
</commit_message>
<xml_diff>
--- a/PAM/caseTest.xlsx
+++ b/PAM/caseTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlsahlen1/Documents/Universitet/Y/TATA62/profit_decomposition/PAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4D5F69-D9A8-3643-B486-748DEF634FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA4AE7C-E65E-9641-ABAC-CE47B55742B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19720" yWindow="-3600" windowWidth="19720" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="procurement" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
   <si>
     <t>Order date</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>Stool 2</t>
+  </si>
+  <si>
+    <t>AED</t>
   </si>
 </sst>
 </file>
@@ -807,9 +810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView zoomScale="238" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="238" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C3"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4943,7 +4946,7 @@
   <sheetViews>
     <sheetView zoomScale="215" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5086,7 +5089,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>13</v>
@@ -5119,12 +5122,30 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -8101,9 +8122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="241" workbookViewId="0">
+    <sheetView zoomScale="241" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8152,7 +8173,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="6">
-        <v>44797</v>
+        <v>44775</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
@@ -12206,7 +12227,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="355" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D2" sqref="D2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12317,7 +12338,7 @@
         <v>44774</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5">
         <v>250000</v>
@@ -16348,7 +16369,7 @@
   <sheetViews>
     <sheetView zoomScale="230" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -22410,7 +22431,7 @@
   <dimension ref="B2:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B2" sqref="B2:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>